<commit_message>
Added more visual ideas
</commit_message>
<xml_diff>
--- a/Dashboard_Draft.xlsx
+++ b/Dashboard_Draft.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitashagill/Desktop/Bootcamp/Weather_Impact_On_Crime_Rates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D34D42-271B-5841-8411-87B82D451EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75661609-6DEB-3345-8D3C-6DCB945AEE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{63BDC5D7-EA13-3843-AC7F-053540A29877}"/>
+    <workbookView xWindow="34540" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{63BDC5D7-EA13-3843-AC7F-053540A29877}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Draft" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -590,7 +590,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>